<commit_message>
Update Excel power network
</commit_message>
<xml_diff>
--- a/Mini-projet-trey_Buchser_Joye/Données/trey_power_network.xlsx
+++ b/Mini-projet-trey_Buchser_Joye/Données/trey_power_network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\matthjoye\github\rhtlab_MIB\Mini-projet-trey_Buchser_Joye\Données\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B325E0AE-879B-45AA-9E48-CAC5DFDDD28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046C34BF-E7E3-4CF7-BB27-15ECDCEAC4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -761,7 +761,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,6 +797,9 @@
       <c r="B2" t="s">
         <v>68</v>
       </c>
+      <c r="C2">
+        <v>0.42</v>
+      </c>
       <c r="D2" t="s">
         <v>80</v>
       </c>
@@ -811,6 +814,9 @@
       <c r="B3" t="s">
         <v>70</v>
       </c>
+      <c r="C3">
+        <v>0.42</v>
+      </c>
       <c r="D3" t="s">
         <v>80</v>
       </c>
@@ -825,6 +831,9 @@
       <c r="B4" t="s">
         <v>71</v>
       </c>
+      <c r="C4">
+        <v>0.42</v>
+      </c>
       <c r="D4" t="s">
         <v>80</v>
       </c>
@@ -839,6 +848,9 @@
       <c r="B5" t="s">
         <v>72</v>
       </c>
+      <c r="C5">
+        <v>0.42</v>
+      </c>
       <c r="D5" t="s">
         <v>80</v>
       </c>
@@ -853,6 +865,9 @@
       <c r="B6" t="s">
         <v>73</v>
       </c>
+      <c r="C6">
+        <v>0.42</v>
+      </c>
       <c r="D6" t="s">
         <v>80</v>
       </c>
@@ -867,6 +882,9 @@
       <c r="B7" t="s">
         <v>74</v>
       </c>
+      <c r="C7">
+        <v>0.42</v>
+      </c>
       <c r="D7" t="s">
         <v>80</v>
       </c>
@@ -881,6 +899,9 @@
       <c r="B8" t="s">
         <v>75</v>
       </c>
+      <c r="C8">
+        <v>0.42</v>
+      </c>
       <c r="D8" t="s">
         <v>80</v>
       </c>
@@ -895,6 +916,9 @@
       <c r="B9" t="s">
         <v>76</v>
       </c>
+      <c r="C9">
+        <v>0.42</v>
+      </c>
       <c r="D9" t="s">
         <v>80</v>
       </c>
@@ -909,6 +933,9 @@
       <c r="B10" t="s">
         <v>77</v>
       </c>
+      <c r="C10">
+        <v>0.42</v>
+      </c>
       <c r="D10" t="s">
         <v>80</v>
       </c>
@@ -923,6 +950,9 @@
       <c r="B11" t="s">
         <v>78</v>
       </c>
+      <c r="C11">
+        <v>0.42</v>
+      </c>
       <c r="D11" t="s">
         <v>80</v>
       </c>
@@ -937,6 +967,9 @@
       <c r="B12" t="s">
         <v>79</v>
       </c>
+      <c r="C12">
+        <v>0.42</v>
+      </c>
       <c r="D12" t="s">
         <v>80</v>
       </c>
@@ -951,6 +984,9 @@
       <c r="B13" s="5" t="s">
         <v>96</v>
       </c>
+      <c r="C13">
+        <v>0.42</v>
+      </c>
       <c r="D13" t="s">
         <v>80</v>
       </c>
@@ -964,6 +1000,9 @@
       </c>
       <c r="B14" t="s">
         <v>97</v>
+      </c>
+      <c r="C14">
+        <v>18.3</v>
       </c>
       <c r="D14" t="s">
         <v>69</v>
@@ -1072,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D466C24-507B-41DF-96AE-5E0A3D434556}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1576,7 +1615,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2081,7 +2120,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2140,7 +2179,9 @@
       <c r="B2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -2316,7 +2357,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2537,7 +2578,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>